<commit_message>
test cases modified to include explicity waits
</commit_message>
<xml_diff>
--- a/testdata/Runtimedata.xlsx
+++ b/testdata/Runtimedata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Hard region</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Retail</t>
   </si>
   <si>
-    <t>R3</t>
+    <t>GK</t>
   </si>
   <si>
     <t>Network</t>
@@ -40,79 +40,82 @@
     <t>Revenue type</t>
   </si>
   <si>
-    <t>7M</t>
+    <t>WQ</t>
   </si>
   <si>
     <t>Commodity code</t>
   </si>
   <si>
-    <t>BQ</t>
+    <t>T0</t>
   </si>
   <si>
     <t>Salesperson</t>
   </si>
   <si>
-    <t>3XW</t>
+    <t>8U0</t>
   </si>
   <si>
     <t>Sales Office</t>
   </si>
   <si>
-    <t>OI</t>
+    <t>FY</t>
   </si>
   <si>
     <t>Standard Cust</t>
   </si>
   <si>
-    <t/>
+    <t>B2</t>
   </si>
   <si>
     <t>Agency Cust</t>
   </si>
   <si>
-    <t>B2</t>
+    <t>8O</t>
   </si>
   <si>
     <t>Rep Cust</t>
   </si>
   <si>
-    <t>Z4</t>
-  </si>
-  <si>
-    <t>3W</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>8O</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>8U0</t>
-  </si>
-  <si>
-    <t>O3</t>
-  </si>
-  <si>
-    <t>N2</t>
-  </si>
-  <si>
-    <t>UG</t>
-  </si>
-  <si>
-    <t>5U</t>
-  </si>
-  <si>
     <t>KC</t>
   </si>
   <si>
-    <t>QU</t>
-  </si>
-  <si>
-    <t>GI</t>
+    <t>Ad copy</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>5D</t>
+  </si>
+  <si>
+    <t>JK</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>KN3</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>0I</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>3V</t>
+  </si>
+  <si>
+    <t>9M</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>XB</t>
   </si>
 </sst>
 </file>
@@ -1047,15 +1050,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.2857142857143"/>
+    <col min="1" max="1" customWidth="true" width="17.3904761904762"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1063,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1079,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1092,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1100,7 +1103,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1108,7 +1111,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1116,7 +1119,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1132,7 +1135,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1140,7 +1143,15 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test cases sync issue fixed
</commit_message>
<xml_diff>
--- a/testdata/Runtimedata.xlsx
+++ b/testdata/Runtimedata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7200"/>
+    <workbookView windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -14,24 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Hard region</t>
   </si>
   <si>
-    <t>9M</t>
+    <t>SS</t>
   </si>
   <si>
     <t>Soft region</t>
   </si>
   <si>
-    <t>ZY</t>
+    <t>74</t>
   </si>
   <si>
     <t>Retail</t>
   </si>
   <si>
-    <t>3V</t>
+    <t>7Q</t>
   </si>
   <si>
     <t>Network</t>
@@ -40,85 +40,97 @@
     <t>Revenue type</t>
   </si>
   <si>
-    <t>W7</t>
+    <t>HF</t>
   </si>
   <si>
     <t>Commodity code</t>
   </si>
   <si>
-    <t>VQ</t>
+    <t>CI</t>
   </si>
   <si>
     <t>Salesperson</t>
   </si>
   <si>
-    <t>QSW</t>
+    <t>U4T</t>
   </si>
   <si>
     <t>Sales Office</t>
   </si>
   <si>
+    <t>I6</t>
+  </si>
+  <si>
+    <t>Standard Cust</t>
+  </si>
+  <si>
+    <t>6D</t>
+  </si>
+  <si>
+    <t>Agency Cust</t>
+  </si>
+  <si>
+    <t>8O</t>
+  </si>
+  <si>
+    <t>Rep Cust</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>Ad copy</t>
+  </si>
+  <si>
     <t>WI</t>
   </si>
   <si>
-    <t>Standard Cust</t>
-  </si>
-  <si>
-    <t>GM</t>
-  </si>
-  <si>
-    <t>Agency Cust</t>
-  </si>
-  <si>
-    <t>8O</t>
-  </si>
-  <si>
-    <t>Rep Cust</t>
-  </si>
-  <si>
-    <t>KC</t>
-  </si>
-  <si>
-    <t>Ad copy</t>
-  </si>
-  <si>
-    <t>5P</t>
-  </si>
-  <si>
-    <t>7DI</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>9X</t>
-  </si>
-  <si>
-    <t>DK</t>
-  </si>
-  <si>
-    <t>OVX</t>
-  </si>
-  <si>
-    <t>0J</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>16</t>
+    <t>H08</t>
+  </si>
+  <si>
+    <t>6V</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>9H</t>
+  </si>
+  <si>
+    <t>ZK</t>
+  </si>
+  <si>
+    <t>2F</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>W4</t>
+  </si>
+  <si>
+    <t>OXU</t>
+  </si>
+  <si>
+    <t>WH</t>
+  </si>
+  <si>
+    <t>1V</t>
+  </si>
+  <si>
+    <t>5C</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>9K</t>
+  </si>
+  <si>
+    <t>J8</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1068,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1069,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1077,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1085,7 +1097,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1098,7 +1110,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1106,7 +1118,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1114,7 +1126,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1122,7 +1134,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1130,7 +1142,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1154,7 +1166,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fluentwait added to wait for file to download completely
</commit_message>
<xml_diff>
--- a/testdata/Runtimedata.xlsx
+++ b/testdata/Runtimedata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Hard region</t>
   </si>
@@ -113,6 +113,27 @@
   </si>
   <si>
     <t>E5</t>
+  </si>
+  <si>
+    <t>NGJ</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>UR</t>
+  </si>
+  <si>
+    <t>0O</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>0Z</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1092,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1079,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1092,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1100,7 +1121,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1108,7 +1129,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1116,7 +1137,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1156,7 +1177,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Afshan branch v01 (#17)
* updating from main (#15)

* Git ignore file updated (#13)

* Git ignore file updated (#14)

* Fluentwait added to wait for file to download completely
</commit_message>
<xml_diff>
--- a/testdata/Runtimedata.xlsx
+++ b/testdata/Runtimedata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Hard region</t>
   </si>
@@ -113,6 +113,27 @@
   </si>
   <si>
     <t>E5</t>
+  </si>
+  <si>
+    <t>NGJ</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>UR</t>
+  </si>
+  <si>
+    <t>0O</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>0Z</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1092,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1079,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1092,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1100,7 +1121,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1108,7 +1129,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1116,7 +1137,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1156,7 +1177,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated selenium to 4.8 fixed older test cases
</commit_message>
<xml_diff>
--- a/testdata/Runtimedata.xlsx
+++ b/testdata/Runtimedata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Hard region</t>
   </si>
@@ -134,6 +134,168 @@
   </si>
   <si>
     <t>0Z</t>
+  </si>
+  <si>
+    <t>VHR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>0W</t>
+  </si>
+  <si>
+    <t>6Z</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>YU</t>
+  </si>
+  <si>
+    <t>VO</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>LZ</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>LY</t>
+  </si>
+  <si>
+    <t>72X</t>
+  </si>
+  <si>
+    <t>6V</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>7DG</t>
+  </si>
+  <si>
+    <t>ZL</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>XK</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>9C</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>L63</t>
+  </si>
+  <si>
+    <t>CC6</t>
+  </si>
+  <si>
+    <t>09B</t>
+  </si>
+  <si>
+    <t>5YW</t>
+  </si>
+  <si>
+    <t>3DY</t>
+  </si>
+  <si>
+    <t>LZQ</t>
+  </si>
+  <si>
+    <t>597</t>
+  </si>
+  <si>
+    <t>6VF</t>
+  </si>
+  <si>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>O4</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>TZ</t>
+  </si>
+  <si>
+    <t>YD</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>OBM</t>
+  </si>
+  <si>
+    <t>KA1</t>
+  </si>
+  <si>
+    <t>GL1</t>
+  </si>
+  <si>
+    <t>ST</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1100,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1113,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1121,7 +1283,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1129,7 +1291,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1137,7 +1299,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1145,7 +1307,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1169,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -1177,7 +1339,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SP and Comodity path Changes in Customer page
</commit_message>
<xml_diff>
--- a/testdata/Runtimedata.xlsx
+++ b/testdata/Runtimedata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D Drive\XGLFinal_Mine\XGLFinal_Mine\testdata\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Hard region</t>
   </si>
@@ -101,12 +101,22 @@
   </si>
   <si>
     <t>LineNumber</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>HNP9Y</t>
+  </si>
+  <si>
+    <t>R8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -421,8 +431,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.42578125"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -491,7 +501,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -515,7 +525,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2">

</xml_diff>

<commit_message>
Ad copy Length fixed 30s
Ad copy Length fixed 30s
</commit_message>
<xml_diff>
--- a/testdata/Runtimedata.xlsx
+++ b/testdata/Runtimedata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Hard region</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>R8</t>
+  </si>
+  <si>
+    <t>8P</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2">

</xml_diff>